<commit_message>
Magiesystem + Shop; viele Änderungen und Bugfixes
</commit_message>
<xml_diff>
--- a/snn/small_gear.xlsx
+++ b/snn/small_gear.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\secure\snn\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="60" windowWidth="18915" windowHeight="10545"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="94">
   <si>
     <t>HM</t>
   </si>
@@ -196,12 +201,114 @@
   </si>
   <si>
     <t>Ranger Arms SM-3</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>melee</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>1M</t>
+  </si>
+  <si>
+    <t>3M</t>
+  </si>
+  <si>
+    <t>2M</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>1S</t>
+  </si>
+  <si>
+    <t>Centurion Laseraxt</t>
+  </si>
+  <si>
+    <t>Cougar Fineblade lang</t>
+  </si>
+  <si>
+    <t>Katana</t>
+  </si>
+  <si>
+    <t>Schwert</t>
+  </si>
+  <si>
+    <t>Streitaxt</t>
+  </si>
+  <si>
+    <t>Unterarmschnappklingen</t>
+  </si>
+  <si>
+    <t>Vibromesser</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>Keule mit Spitzen</t>
+  </si>
+  <si>
+    <t>Claymore</t>
+  </si>
+  <si>
+    <t>Schicke Lederklamotte</t>
+  </si>
+  <si>
+    <t>Echtleder Kleidung</t>
+  </si>
+  <si>
+    <t>Panzerjacke</t>
+  </si>
+  <si>
+    <t>Panzerweste</t>
+  </si>
+  <si>
+    <t>Gefütterter Mantel</t>
+  </si>
+  <si>
+    <t>Leichter Sicherheitspanzer</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>armor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -680,7 +787,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -690,7 +797,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -698,7 +804,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -706,7 +811,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -714,7 +818,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -772,14 +875,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -817,9 +923,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -852,9 +958,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -887,9 +1010,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1063,20 +1203,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R21"/>
+  <dimension ref="A1:U35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="I16" workbookViewId="0">
+      <selection activeCell="S1" sqref="S1:U35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.86328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="34.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -1102,8 +1242,44 @@
       <c r="I1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J1">
+        <v>0</v>
+      </c>
+      <c r="K1">
+        <v>0</v>
+      </c>
+      <c r="L1">
+        <v>0</v>
+      </c>
+      <c r="M1" s="13">
+        <v>0</v>
+      </c>
+      <c r="N1" s="13">
+        <v>0</v>
+      </c>
+      <c r="O1" s="13">
+        <v>0</v>
+      </c>
+      <c r="P1" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q1" s="13">
+        <v>0</v>
+      </c>
+      <c r="R1" s="13">
+        <v>0</v>
+      </c>
+      <c r="S1" s="13">
+        <v>0</v>
+      </c>
+      <c r="T1" s="13">
+        <v>0</v>
+      </c>
+      <c r="U1" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -1120,7 +1296,7 @@
         <v>2</v>
       </c>
       <c r="F2" s="3">
-        <v>750</v>
+        <v>1050</v>
       </c>
       <c r="G2" s="1">
         <v>1</v>
@@ -1128,11 +1304,47 @@
       <c r="H2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="I2" s="10" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J2" s="13">
+        <v>0</v>
+      </c>
+      <c r="K2" s="13">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2" s="13">
+        <v>0</v>
+      </c>
+      <c r="N2" s="13">
+        <v>0</v>
+      </c>
+      <c r="O2" s="13">
+        <v>0</v>
+      </c>
+      <c r="P2" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="13">
+        <v>0</v>
+      </c>
+      <c r="R2" s="13">
+        <v>0</v>
+      </c>
+      <c r="S2" s="13">
+        <v>0</v>
+      </c>
+      <c r="T2" s="13">
+        <v>0</v>
+      </c>
+      <c r="U2" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -1155,11 +1367,47 @@
       <c r="H3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="I3" s="10" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J3" s="13">
+        <v>0</v>
+      </c>
+      <c r="K3" s="13">
+        <v>0</v>
+      </c>
+      <c r="L3" s="13">
+        <v>0</v>
+      </c>
+      <c r="M3" s="13">
+        <v>0</v>
+      </c>
+      <c r="N3" s="13">
+        <v>0</v>
+      </c>
+      <c r="O3" s="13">
+        <v>0</v>
+      </c>
+      <c r="P3" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="13">
+        <v>0</v>
+      </c>
+      <c r="R3" s="13">
+        <v>0</v>
+      </c>
+      <c r="S3" s="13">
+        <v>0</v>
+      </c>
+      <c r="T3" s="13">
+        <v>0</v>
+      </c>
+      <c r="U3" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
@@ -1174,7 +1422,7 @@
         <v>2</v>
       </c>
       <c r="F4" s="3">
-        <v>1150</v>
+        <v>2500</v>
       </c>
       <c r="G4" s="1">
         <v>0</v>
@@ -1182,11 +1430,47 @@
       <c r="H4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I4" s="12" t="s">
+      <c r="I4" s="10" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J4" s="13">
+        <v>0</v>
+      </c>
+      <c r="K4" s="13">
+        <v>0</v>
+      </c>
+      <c r="L4" s="13">
+        <v>0</v>
+      </c>
+      <c r="M4" s="13">
+        <v>0</v>
+      </c>
+      <c r="N4" s="13">
+        <v>0</v>
+      </c>
+      <c r="O4" s="13">
+        <v>0</v>
+      </c>
+      <c r="P4" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="13">
+        <v>0</v>
+      </c>
+      <c r="R4" s="13">
+        <v>0</v>
+      </c>
+      <c r="S4" s="13">
+        <v>0</v>
+      </c>
+      <c r="T4" s="13">
+        <v>0</v>
+      </c>
+      <c r="U4" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -1211,27 +1495,63 @@
       <c r="H5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I5" s="12" t="s">
+      <c r="I5" s="10" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J5" s="13">
+        <v>0</v>
+      </c>
+      <c r="K5" s="13">
+        <v>0</v>
+      </c>
+      <c r="L5" s="13">
+        <v>0</v>
+      </c>
+      <c r="M5" s="13">
+        <v>0</v>
+      </c>
+      <c r="N5" s="13">
+        <v>0</v>
+      </c>
+      <c r="O5" s="13">
+        <v>0</v>
+      </c>
+      <c r="P5" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="13">
+        <v>0</v>
+      </c>
+      <c r="R5" s="13">
+        <v>0</v>
+      </c>
+      <c r="S5" s="13">
+        <v>0</v>
+      </c>
+      <c r="T5" s="13">
+        <v>0</v>
+      </c>
+      <c r="U5" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="E6" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="F6" s="7">
+      <c r="E6" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" s="6">
         <v>650</v>
       </c>
       <c r="G6">
@@ -1243,33 +1563,60 @@
       <c r="I6" t="s">
         <v>35</v>
       </c>
-      <c r="J6" s="6"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="5"/>
-      <c r="P6" s="4"/>
-      <c r="Q6" s="4"/>
-      <c r="R6" s="4"/>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J6" s="13">
+        <v>0</v>
+      </c>
+      <c r="K6" s="13">
+        <v>0</v>
+      </c>
+      <c r="L6" s="13">
+        <v>0</v>
+      </c>
+      <c r="M6" s="13">
+        <v>0</v>
+      </c>
+      <c r="N6" s="13">
+        <v>0</v>
+      </c>
+      <c r="O6" s="13">
+        <v>0</v>
+      </c>
+      <c r="P6" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="13">
+        <v>0</v>
+      </c>
+      <c r="R6" s="13">
+        <v>0</v>
+      </c>
+      <c r="S6" s="13">
+        <v>0</v>
+      </c>
+      <c r="T6" s="13">
+        <v>0</v>
+      </c>
+      <c r="U6" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="F7" s="7">
+      <c r="E7" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F7" s="6">
         <v>450</v>
       </c>
       <c r="G7">
@@ -1278,36 +1625,63 @@
       <c r="H7" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="I7" s="12" t="s">
+      <c r="I7" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="J7" s="6"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="5"/>
-      <c r="P7" s="4"/>
-      <c r="Q7" s="4"/>
-      <c r="R7" s="4"/>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J7" s="13">
+        <v>0</v>
+      </c>
+      <c r="K7" s="13">
+        <v>0</v>
+      </c>
+      <c r="L7" s="13">
+        <v>0</v>
+      </c>
+      <c r="M7" s="13">
+        <v>0</v>
+      </c>
+      <c r="N7" s="13">
+        <v>0</v>
+      </c>
+      <c r="O7" s="13">
+        <v>0</v>
+      </c>
+      <c r="P7" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="13">
+        <v>0</v>
+      </c>
+      <c r="R7" s="13">
+        <v>0</v>
+      </c>
+      <c r="S7" s="13">
+        <v>0</v>
+      </c>
+      <c r="T7" s="13">
+        <v>0</v>
+      </c>
+      <c r="U7" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A8" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="F8" s="7">
+      <c r="E8" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F8" s="6">
         <v>425</v>
       </c>
       <c r="G8">
@@ -1316,36 +1690,63 @@
       <c r="H8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="12" t="s">
+      <c r="I8" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="J8" s="6"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="5"/>
-      <c r="P8" s="4"/>
-      <c r="Q8" s="4"/>
-      <c r="R8" s="4"/>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J8" s="13">
+        <v>0</v>
+      </c>
+      <c r="K8" s="13">
+        <v>0</v>
+      </c>
+      <c r="L8" s="13">
+        <v>0</v>
+      </c>
+      <c r="M8" s="13">
+        <v>0</v>
+      </c>
+      <c r="N8" s="13">
+        <v>0</v>
+      </c>
+      <c r="O8" s="13">
+        <v>0</v>
+      </c>
+      <c r="P8" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="13">
+        <v>0</v>
+      </c>
+      <c r="R8" s="13">
+        <v>0</v>
+      </c>
+      <c r="S8" s="13">
+        <v>0</v>
+      </c>
+      <c r="T8" s="13">
+        <v>0</v>
+      </c>
+      <c r="U8" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A9" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="F9" s="7">
+      <c r="E9" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F9" s="6">
         <v>2300</v>
       </c>
       <c r="G9">
@@ -1354,37 +1755,64 @@
       <c r="H9" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="I9" s="12" t="s">
+      <c r="I9" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="J9" s="6"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="4"/>
-      <c r="O9" s="5"/>
-      <c r="P9" s="4"/>
-      <c r="Q9" s="4"/>
-      <c r="R9" s="4"/>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J9" s="13">
+        <v>0</v>
+      </c>
+      <c r="K9" s="13">
+        <v>0</v>
+      </c>
+      <c r="L9" s="13">
+        <v>0</v>
+      </c>
+      <c r="M9" s="13">
+        <v>0</v>
+      </c>
+      <c r="N9" s="13">
+        <v>0</v>
+      </c>
+      <c r="O9" s="13">
+        <v>0</v>
+      </c>
+      <c r="P9" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="13">
+        <v>0</v>
+      </c>
+      <c r="R9" s="13">
+        <v>0</v>
+      </c>
+      <c r="S9" s="13">
+        <v>0</v>
+      </c>
+      <c r="T9" s="13">
+        <v>0</v>
+      </c>
+      <c r="U9" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A10" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="F10" s="7">
-        <v>300</v>
+      <c r="E10" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F10" s="6">
+        <v>600</v>
       </c>
       <c r="G10">
         <v>0</v>
@@ -1392,37 +1820,64 @@
       <c r="H10" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="I10" s="12" t="s">
+      <c r="I10" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="J10" s="6"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
-      <c r="N10" s="4"/>
-      <c r="O10" s="5"/>
-      <c r="P10" s="4"/>
-      <c r="Q10" s="4"/>
-      <c r="R10" s="4"/>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J10" s="13">
+        <v>0</v>
+      </c>
+      <c r="K10" s="13">
+        <v>0</v>
+      </c>
+      <c r="L10" s="13">
+        <v>0</v>
+      </c>
+      <c r="M10" s="13">
+        <v>0</v>
+      </c>
+      <c r="N10" s="13">
+        <v>0</v>
+      </c>
+      <c r="O10" s="13">
+        <v>0</v>
+      </c>
+      <c r="P10" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="13">
+        <v>0</v>
+      </c>
+      <c r="R10" s="13">
+        <v>0</v>
+      </c>
+      <c r="S10" s="13">
+        <v>0</v>
+      </c>
+      <c r="T10" s="13">
+        <v>0</v>
+      </c>
+      <c r="U10" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A11" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="F11" s="7">
-        <v>900</v>
+      <c r="F11" s="6">
+        <v>1800</v>
       </c>
       <c r="G11">
         <v>2</v>
@@ -1430,398 +1885,1482 @@
       <c r="H11" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="I11" s="12" t="s">
+      <c r="I11" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
-      <c r="N11" s="4"/>
-      <c r="O11" s="5"/>
-      <c r="P11" s="4"/>
-      <c r="Q11" s="4"/>
-      <c r="R11" s="4"/>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+      <c r="J11" s="13">
+        <v>0</v>
+      </c>
+      <c r="K11" s="13">
+        <v>0</v>
+      </c>
+      <c r="L11" s="13">
+        <v>0</v>
+      </c>
+      <c r="M11" s="13">
+        <v>0</v>
+      </c>
+      <c r="N11" s="13">
+        <v>0</v>
+      </c>
+      <c r="O11" s="13">
+        <v>0</v>
+      </c>
+      <c r="P11" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="13">
+        <v>0</v>
+      </c>
+      <c r="R11" s="13">
+        <v>0</v>
+      </c>
+      <c r="S11" s="13">
+        <v>0</v>
+      </c>
+      <c r="T11" s="13">
+        <v>0</v>
+      </c>
+      <c r="U11" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A12" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="D12" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="E12" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="F12" s="11">
-        <v>1200</v>
+      <c r="F12" s="9">
+        <v>2000</v>
       </c>
       <c r="G12">
         <v>1</v>
       </c>
-      <c r="H12" s="8" t="s">
+      <c r="H12" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="I12" s="12" t="s">
+      <c r="I12" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="J12" s="10"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="8"/>
-      <c r="M12" s="8"/>
-      <c r="N12" s="8"/>
-      <c r="O12" s="9"/>
-      <c r="P12" s="8"/>
-      <c r="Q12" s="8"/>
-      <c r="R12" s="8"/>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" s="12" t="s">
+      <c r="J12" s="13">
+        <v>0</v>
+      </c>
+      <c r="K12" s="13">
+        <v>0</v>
+      </c>
+      <c r="L12" s="13">
+        <v>0</v>
+      </c>
+      <c r="M12" s="13">
+        <v>0</v>
+      </c>
+      <c r="N12" s="13">
+        <v>0</v>
+      </c>
+      <c r="O12" s="13">
+        <v>0</v>
+      </c>
+      <c r="P12" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="13">
+        <v>0</v>
+      </c>
+      <c r="R12" s="13">
+        <v>0</v>
+      </c>
+      <c r="S12" s="13">
+        <v>0</v>
+      </c>
+      <c r="T12" s="13">
+        <v>0</v>
+      </c>
+      <c r="U12" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A13" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="B13" s="14">
+      <c r="B13" s="11">
         <v>30</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="D13" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="E13" s="14" t="s">
+      <c r="E13" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="F13" s="15">
-        <v>800</v>
+      <c r="F13" s="12">
+        <v>1000</v>
       </c>
       <c r="G13">
         <v>1</v>
       </c>
-      <c r="H13" s="12" t="s">
+      <c r="H13" s="10" t="s">
         <v>15</v>
       </c>
       <c r="I13" t="s">
         <v>34</v>
       </c>
-      <c r="J13" s="14"/>
-      <c r="K13" s="12"/>
-      <c r="L13" s="12"/>
-      <c r="M13" s="12"/>
-      <c r="N13" s="12"/>
-      <c r="O13" s="13"/>
-      <c r="P13" s="12"/>
-      <c r="Q13" s="12"/>
-      <c r="R13" s="12"/>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A14" s="12" t="s">
+      <c r="J13" s="13">
+        <v>0</v>
+      </c>
+      <c r="K13" s="13">
+        <v>0</v>
+      </c>
+      <c r="L13" s="13">
+        <v>0</v>
+      </c>
+      <c r="M13" s="13">
+        <v>0</v>
+      </c>
+      <c r="N13" s="13">
+        <v>0</v>
+      </c>
+      <c r="O13" s="13">
+        <v>0</v>
+      </c>
+      <c r="P13" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="13">
+        <v>0</v>
+      </c>
+      <c r="R13" s="13">
+        <v>0</v>
+      </c>
+      <c r="S13" s="13">
+        <v>0</v>
+      </c>
+      <c r="T13" s="13">
+        <v>0</v>
+      </c>
+      <c r="U13" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A14" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="14">
+      <c r="B14" s="11">
         <v>32</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="D14" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="E14" s="14" t="s">
+      <c r="E14" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="F14" s="15">
-        <v>850</v>
+      <c r="F14" s="12">
+        <v>1700</v>
       </c>
       <c r="G14">
         <v>3</v>
       </c>
-      <c r="H14" s="12" t="s">
+      <c r="H14" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="I14" s="12" t="s">
+      <c r="I14" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="J14" s="14"/>
-      <c r="K14" s="12"/>
-      <c r="L14" s="12"/>
-      <c r="M14" s="12"/>
-      <c r="N14" s="12"/>
-      <c r="O14" s="13"/>
-      <c r="P14" s="12"/>
-      <c r="Q14" s="12"/>
-      <c r="R14" s="12"/>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15" s="12" t="s">
+      <c r="J14" s="13">
+        <v>0</v>
+      </c>
+      <c r="K14" s="13">
+        <v>0</v>
+      </c>
+      <c r="L14" s="13">
+        <v>0</v>
+      </c>
+      <c r="M14" s="13">
+        <v>0</v>
+      </c>
+      <c r="N14" s="13">
+        <v>0</v>
+      </c>
+      <c r="O14" s="13">
+        <v>0</v>
+      </c>
+      <c r="P14" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="13">
+        <v>0</v>
+      </c>
+      <c r="R14" s="13">
+        <v>0</v>
+      </c>
+      <c r="S14" s="13">
+        <v>0</v>
+      </c>
+      <c r="T14" s="13">
+        <v>0</v>
+      </c>
+      <c r="U14" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A15" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="14">
+      <c r="B15" s="11">
         <v>28</v>
       </c>
-      <c r="C15" s="14" t="s">
+      <c r="C15" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D15" s="14" t="s">
+      <c r="D15" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="E15" s="14" t="s">
+      <c r="E15" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="F15" s="15">
-        <v>1200</v>
+      <c r="F15" s="12">
+        <v>2400</v>
       </c>
       <c r="G15">
         <v>3</v>
       </c>
-      <c r="H15" s="12" t="s">
+      <c r="H15" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="I15" s="12" t="s">
+      <c r="I15" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="J15" s="12"/>
-      <c r="K15" s="12"/>
-      <c r="L15" s="12"/>
-      <c r="M15" s="12"/>
-      <c r="N15" s="12"/>
-      <c r="O15" s="13"/>
-      <c r="P15" s="12"/>
-      <c r="Q15" s="12"/>
-      <c r="R15" s="12"/>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" s="12" t="s">
+      <c r="J15" s="13">
+        <v>0</v>
+      </c>
+      <c r="K15" s="13">
+        <v>0</v>
+      </c>
+      <c r="L15" s="13">
+        <v>0</v>
+      </c>
+      <c r="M15" s="13">
+        <v>0</v>
+      </c>
+      <c r="N15" s="13">
+        <v>0</v>
+      </c>
+      <c r="O15" s="13">
+        <v>0</v>
+      </c>
+      <c r="P15" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="13">
+        <v>0</v>
+      </c>
+      <c r="R15" s="13">
+        <v>0</v>
+      </c>
+      <c r="S15" s="13">
+        <v>0</v>
+      </c>
+      <c r="T15" s="13">
+        <v>0</v>
+      </c>
+      <c r="U15" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A16" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="B16" s="14">
+      <c r="B16" s="11">
         <v>36</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="C16" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D16" s="14" t="s">
+      <c r="D16" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="E16" s="14" t="s">
+      <c r="E16" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="F16" s="15">
-        <v>4000</v>
+      <c r="F16" s="12">
+        <v>8000</v>
       </c>
       <c r="G16">
         <v>3</v>
       </c>
-      <c r="H16" s="12" t="s">
+      <c r="H16" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="I16" s="12" t="s">
+      <c r="I16" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="J16" s="12"/>
-      <c r="K16" s="12"/>
-      <c r="L16" s="12"/>
-      <c r="M16" s="12"/>
-      <c r="N16" s="12"/>
-      <c r="O16" s="13"/>
-      <c r="P16" s="12"/>
-      <c r="Q16" s="12"/>
-      <c r="R16" s="12"/>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A17" s="12" t="s">
+      <c r="J16" s="13">
+        <v>0</v>
+      </c>
+      <c r="K16" s="13">
+        <v>0</v>
+      </c>
+      <c r="L16" s="13">
+        <v>0</v>
+      </c>
+      <c r="M16" s="13">
+        <v>0</v>
+      </c>
+      <c r="N16" s="13">
+        <v>0</v>
+      </c>
+      <c r="O16" s="13">
+        <v>0</v>
+      </c>
+      <c r="P16" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="13">
+        <v>0</v>
+      </c>
+      <c r="R16" s="13">
+        <v>0</v>
+      </c>
+      <c r="S16" s="13">
+        <v>0</v>
+      </c>
+      <c r="T16" s="13">
+        <v>0</v>
+      </c>
+      <c r="U16" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A17" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B17" s="14">
+      <c r="B17" s="11">
         <v>32</v>
       </c>
-      <c r="C17" s="14" t="s">
+      <c r="C17" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D17" s="14" t="s">
+      <c r="D17" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="E17" s="14" t="s">
+      <c r="E17" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="F17" s="15">
-        <v>950</v>
+      <c r="F17" s="12">
+        <v>1550</v>
       </c>
       <c r="G17">
         <v>3</v>
       </c>
-      <c r="H17" s="12" t="s">
+      <c r="H17" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="I17" s="12" t="s">
+      <c r="I17" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="J17" s="14"/>
-      <c r="K17" s="12"/>
-      <c r="L17" s="12"/>
-      <c r="M17" s="12"/>
-      <c r="N17" s="12"/>
-      <c r="O17" s="13"/>
-      <c r="P17" s="12"/>
-      <c r="Q17" s="12"/>
-      <c r="R17" s="12"/>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A18" s="12" t="s">
+      <c r="J17" s="13">
+        <v>0</v>
+      </c>
+      <c r="K17" s="13">
+        <v>0</v>
+      </c>
+      <c r="L17" s="13">
+        <v>0</v>
+      </c>
+      <c r="M17" s="13">
+        <v>0</v>
+      </c>
+      <c r="N17" s="13">
+        <v>0</v>
+      </c>
+      <c r="O17" s="13">
+        <v>0</v>
+      </c>
+      <c r="P17" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="13">
+        <v>0</v>
+      </c>
+      <c r="R17" s="13">
+        <v>0</v>
+      </c>
+      <c r="S17" s="13">
+        <v>0</v>
+      </c>
+      <c r="T17" s="13">
+        <v>0</v>
+      </c>
+      <c r="U17" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A18" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="B18" s="14">
+      <c r="B18" s="11">
         <v>30</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D18" s="14" t="s">
+      <c r="D18" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="E18" s="14" t="s">
+      <c r="E18" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="F18" s="15">
-        <v>650</v>
+      <c r="F18" s="12">
+        <v>850</v>
       </c>
       <c r="G18">
         <v>0</v>
       </c>
-      <c r="H18" s="12" t="s">
+      <c r="H18" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="I18" s="12" t="s">
+      <c r="I18" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="J18" s="14"/>
-      <c r="K18" s="12"/>
-      <c r="L18" s="12"/>
-      <c r="M18" s="12"/>
-      <c r="N18" s="12"/>
-      <c r="O18" s="13"/>
-      <c r="P18" s="12"/>
-      <c r="Q18" s="12"/>
-      <c r="R18" s="12"/>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A19" s="16" t="s">
+      <c r="J18" s="13">
+        <v>0</v>
+      </c>
+      <c r="K18" s="13">
+        <v>0</v>
+      </c>
+      <c r="L18" s="13">
+        <v>0</v>
+      </c>
+      <c r="M18" s="13">
+        <v>0</v>
+      </c>
+      <c r="N18" s="13">
+        <v>0</v>
+      </c>
+      <c r="O18" s="13">
+        <v>0</v>
+      </c>
+      <c r="P18" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="13">
+        <v>0</v>
+      </c>
+      <c r="R18" s="13">
+        <v>0</v>
+      </c>
+      <c r="S18" s="13">
+        <v>0</v>
+      </c>
+      <c r="T18" s="13">
+        <v>0</v>
+      </c>
+      <c r="U18" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A19" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="B19" s="18">
+      <c r="B19" s="14">
         <v>5</v>
       </c>
-      <c r="C19" s="18" t="s">
+      <c r="C19" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="D19" s="18" t="s">
+      <c r="D19" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="E19" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="F19" s="19">
+      <c r="E19" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="F19" s="15">
         <v>800</v>
       </c>
       <c r="G19">
         <v>0</v>
       </c>
-      <c r="H19" s="16" t="s">
+      <c r="H19" s="13" t="s">
         <v>15</v>
       </c>
       <c r="I19" t="s">
         <v>56</v>
       </c>
-      <c r="J19" s="18"/>
-      <c r="K19" s="16"/>
-      <c r="L19" s="16"/>
-      <c r="M19" s="16"/>
-      <c r="N19" s="16"/>
-      <c r="O19" s="17"/>
-      <c r="P19" s="16"/>
-      <c r="Q19" s="16"/>
-      <c r="R19" s="16"/>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A20" s="16" t="s">
+      <c r="J19" s="13">
+        <v>0</v>
+      </c>
+      <c r="K19" s="13">
+        <v>0</v>
+      </c>
+      <c r="L19" s="13">
+        <v>0</v>
+      </c>
+      <c r="M19" s="13">
+        <v>0</v>
+      </c>
+      <c r="N19" s="13">
+        <v>0</v>
+      </c>
+      <c r="O19" s="13">
+        <v>0</v>
+      </c>
+      <c r="P19" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="13">
+        <v>0</v>
+      </c>
+      <c r="R19" s="13">
+        <v>0</v>
+      </c>
+      <c r="S19" s="13">
+        <v>0</v>
+      </c>
+      <c r="T19" s="13">
+        <v>0</v>
+      </c>
+      <c r="U19" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A20" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="B20" s="18">
+      <c r="B20" s="14">
         <v>5</v>
       </c>
-      <c r="C20" s="18" t="s">
+      <c r="C20" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="D20" s="18" t="s">
+      <c r="D20" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="E20" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="F20" s="19">
+      <c r="E20" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="F20" s="15">
         <v>1300</v>
       </c>
       <c r="G20">
         <v>0</v>
       </c>
-      <c r="H20" s="16" t="s">
+      <c r="H20" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="I20" s="16" t="s">
+      <c r="I20" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="J20" s="18"/>
-      <c r="K20" s="16"/>
-      <c r="L20" s="16"/>
-      <c r="M20" s="16"/>
-      <c r="N20" s="16"/>
-      <c r="O20" s="17"/>
-      <c r="P20" s="16"/>
-      <c r="Q20" s="16"/>
-      <c r="R20" s="16"/>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A21" s="16" t="s">
+      <c r="J20" s="13">
+        <v>0</v>
+      </c>
+      <c r="K20" s="13">
+        <v>0</v>
+      </c>
+      <c r="L20" s="13">
+        <v>0</v>
+      </c>
+      <c r="M20" s="13">
+        <v>0</v>
+      </c>
+      <c r="N20" s="13">
+        <v>0</v>
+      </c>
+      <c r="O20" s="13">
+        <v>0</v>
+      </c>
+      <c r="P20" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="13">
+        <v>0</v>
+      </c>
+      <c r="R20" s="13">
+        <v>0</v>
+      </c>
+      <c r="S20" s="13">
+        <v>0</v>
+      </c>
+      <c r="T20" s="13">
+        <v>0</v>
+      </c>
+      <c r="U20" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A21" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="B21" s="18">
+      <c r="B21" s="14">
         <v>6</v>
       </c>
-      <c r="C21" s="18" t="s">
+      <c r="C21" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="D21" s="18" t="s">
+      <c r="D21" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="E21" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="F21" s="19">
-        <v>4000</v>
+      <c r="E21" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="F21" s="15">
+        <v>12000</v>
       </c>
       <c r="G21">
         <v>2</v>
       </c>
-      <c r="H21" s="16" t="s">
+      <c r="H21" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="I21" s="16" t="s">
+      <c r="I21" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="J21" s="16"/>
-      <c r="K21" s="16"/>
-      <c r="L21" s="16"/>
-      <c r="M21" s="16"/>
-      <c r="N21" s="16"/>
-      <c r="O21" s="17"/>
-      <c r="P21" s="16"/>
-      <c r="Q21" s="16"/>
-      <c r="R21" s="16"/>
+      <c r="J21" s="13">
+        <v>0</v>
+      </c>
+      <c r="K21" s="13">
+        <v>0</v>
+      </c>
+      <c r="L21" s="13">
+        <v>0</v>
+      </c>
+      <c r="M21" s="13">
+        <v>0</v>
+      </c>
+      <c r="N21" s="13">
+        <v>0</v>
+      </c>
+      <c r="O21" s="13">
+        <v>0</v>
+      </c>
+      <c r="P21" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="13">
+        <v>0</v>
+      </c>
+      <c r="R21" s="13">
+        <v>0</v>
+      </c>
+      <c r="S21" s="13">
+        <v>0</v>
+      </c>
+      <c r="T21" s="13">
+        <v>0</v>
+      </c>
+      <c r="U21" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A22" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="E22" s="14"/>
+      <c r="F22" s="15">
+        <v>2500</v>
+      </c>
+      <c r="G22" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="H22" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="I22" s="14"/>
+      <c r="J22" s="13">
+        <v>0</v>
+      </c>
+      <c r="K22" s="14">
+        <v>1</v>
+      </c>
+      <c r="L22" s="13">
+        <v>0</v>
+      </c>
+      <c r="M22" s="13">
+        <v>0</v>
+      </c>
+      <c r="N22" s="13">
+        <v>0</v>
+      </c>
+      <c r="O22" s="13">
+        <v>0</v>
+      </c>
+      <c r="P22" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="13">
+        <v>0</v>
+      </c>
+      <c r="R22" s="13">
+        <v>0</v>
+      </c>
+      <c r="S22" s="13">
+        <v>0</v>
+      </c>
+      <c r="T22" s="13">
+        <v>0</v>
+      </c>
+      <c r="U22" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A23" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="E23" s="14"/>
+      <c r="F23" s="15">
+        <v>1500</v>
+      </c>
+      <c r="G23" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="H23" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="J23" s="13">
+        <v>0</v>
+      </c>
+      <c r="K23" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="L23" s="13">
+        <v>0</v>
+      </c>
+      <c r="M23" s="13">
+        <v>0</v>
+      </c>
+      <c r="N23" s="13">
+        <v>0</v>
+      </c>
+      <c r="O23" s="13">
+        <v>0</v>
+      </c>
+      <c r="P23" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="13">
+        <v>0</v>
+      </c>
+      <c r="R23" s="13">
+        <v>0</v>
+      </c>
+      <c r="S23" s="13">
+        <v>0</v>
+      </c>
+      <c r="T23" s="13">
+        <v>0</v>
+      </c>
+      <c r="U23" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A24" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="E24" s="14"/>
+      <c r="F24" s="15">
+        <v>2000</v>
+      </c>
+      <c r="G24" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="H24" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="J24" s="13">
+        <v>0</v>
+      </c>
+      <c r="K24" s="14">
+        <v>1</v>
+      </c>
+      <c r="L24" s="13">
+        <v>0</v>
+      </c>
+      <c r="M24" s="13">
+        <v>0</v>
+      </c>
+      <c r="N24" s="13">
+        <v>0</v>
+      </c>
+      <c r="O24" s="13">
+        <v>0</v>
+      </c>
+      <c r="P24" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="13">
+        <v>0</v>
+      </c>
+      <c r="R24" s="13">
+        <v>0</v>
+      </c>
+      <c r="S24" s="13">
+        <v>0</v>
+      </c>
+      <c r="T24" s="13">
+        <v>0</v>
+      </c>
+      <c r="U24" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A25" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="E25" s="14"/>
+      <c r="F25" s="15">
+        <v>500</v>
+      </c>
+      <c r="G25" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="H25" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="J25" s="13">
+        <v>0</v>
+      </c>
+      <c r="K25" s="14">
+        <v>1</v>
+      </c>
+      <c r="L25" s="13">
+        <v>0</v>
+      </c>
+      <c r="M25" s="13">
+        <v>0</v>
+      </c>
+      <c r="N25" s="13">
+        <v>0</v>
+      </c>
+      <c r="O25" s="13">
+        <v>0</v>
+      </c>
+      <c r="P25" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q25" s="13">
+        <v>0</v>
+      </c>
+      <c r="R25" s="13">
+        <v>0</v>
+      </c>
+      <c r="S25" s="13">
+        <v>0</v>
+      </c>
+      <c r="T25" s="13">
+        <v>0</v>
+      </c>
+      <c r="U25" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A26" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="E26" s="14"/>
+      <c r="F26" s="15">
+        <v>1000</v>
+      </c>
+      <c r="G26" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="H26" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="J26" s="13">
+        <v>0</v>
+      </c>
+      <c r="K26" s="14">
+        <v>2</v>
+      </c>
+      <c r="L26" s="13">
+        <v>0</v>
+      </c>
+      <c r="M26" s="13">
+        <v>0</v>
+      </c>
+      <c r="N26" s="13">
+        <v>0</v>
+      </c>
+      <c r="O26" s="13">
+        <v>0</v>
+      </c>
+      <c r="P26" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q26" s="13">
+        <v>0</v>
+      </c>
+      <c r="R26" s="13">
+        <v>0</v>
+      </c>
+      <c r="S26" s="13">
+        <v>0</v>
+      </c>
+      <c r="T26" s="13">
+        <v>0</v>
+      </c>
+      <c r="U26" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A27" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="E27" s="14"/>
+      <c r="F27" s="15">
+        <v>1700</v>
+      </c>
+      <c r="G27" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="H27" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="J27" s="13">
+        <v>0</v>
+      </c>
+      <c r="K27" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="L27" s="13">
+        <v>0</v>
+      </c>
+      <c r="M27" s="13">
+        <v>0</v>
+      </c>
+      <c r="N27" s="13">
+        <v>0</v>
+      </c>
+      <c r="O27" s="13">
+        <v>0</v>
+      </c>
+      <c r="P27" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q27" s="13">
+        <v>0</v>
+      </c>
+      <c r="R27" s="13">
+        <v>0</v>
+      </c>
+      <c r="S27" s="13">
+        <v>0</v>
+      </c>
+      <c r="T27" s="13">
+        <v>0</v>
+      </c>
+      <c r="U27" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A28" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="E28" s="14"/>
+      <c r="F28" s="15">
+        <v>2000</v>
+      </c>
+      <c r="G28" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="H28" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="J28" s="13">
+        <v>0</v>
+      </c>
+      <c r="K28" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="L28" s="13">
+        <v>0</v>
+      </c>
+      <c r="M28" s="13">
+        <v>0</v>
+      </c>
+      <c r="N28" s="13">
+        <v>0</v>
+      </c>
+      <c r="O28" s="13">
+        <v>0</v>
+      </c>
+      <c r="P28" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q28" s="13">
+        <v>0</v>
+      </c>
+      <c r="R28" s="13">
+        <v>0</v>
+      </c>
+      <c r="S28" s="13">
+        <v>0</v>
+      </c>
+      <c r="T28" s="13">
+        <v>0</v>
+      </c>
+      <c r="U28" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A29" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="E29" s="14"/>
+      <c r="F29" s="15">
+        <v>750</v>
+      </c>
+      <c r="G29" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="H29" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="I29" s="14"/>
+      <c r="J29" s="13">
+        <v>0</v>
+      </c>
+      <c r="K29" s="14">
+        <v>1</v>
+      </c>
+      <c r="L29" s="13">
+        <v>0</v>
+      </c>
+      <c r="M29" s="13">
+        <v>0</v>
+      </c>
+      <c r="N29" s="13">
+        <v>0</v>
+      </c>
+      <c r="O29" s="13">
+        <v>0</v>
+      </c>
+      <c r="P29" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q29" s="13">
+        <v>0</v>
+      </c>
+      <c r="R29" s="13">
+        <v>0</v>
+      </c>
+      <c r="S29" s="13">
+        <v>0</v>
+      </c>
+      <c r="T29" s="13">
+        <v>0</v>
+      </c>
+      <c r="U29" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A30" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="E30" s="14"/>
+      <c r="F30" s="15">
+        <v>2000</v>
+      </c>
+      <c r="G30" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="H30" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="I30" s="14"/>
+      <c r="J30" s="13">
+        <v>0</v>
+      </c>
+      <c r="K30" s="14">
+        <v>2</v>
+      </c>
+      <c r="L30" s="13">
+        <v>0</v>
+      </c>
+      <c r="M30" s="13">
+        <v>0</v>
+      </c>
+      <c r="N30" s="13">
+        <v>0</v>
+      </c>
+      <c r="O30" s="13">
+        <v>0</v>
+      </c>
+      <c r="P30" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q30" s="13">
+        <v>0</v>
+      </c>
+      <c r="R30" s="13">
+        <v>0</v>
+      </c>
+      <c r="S30" s="13">
+        <v>0</v>
+      </c>
+      <c r="T30" s="13">
+        <v>0</v>
+      </c>
+      <c r="U30" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
+        <v>86</v>
+      </c>
+      <c r="B31" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F31" s="15">
+        <v>750</v>
+      </c>
+      <c r="G31" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="H31" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="J31">
+        <v>2</v>
+      </c>
+      <c r="K31" s="14">
+        <v>0</v>
+      </c>
+      <c r="L31" s="13">
+        <v>0</v>
+      </c>
+      <c r="M31" s="13">
+        <v>0</v>
+      </c>
+      <c r="N31" s="13">
+        <v>0</v>
+      </c>
+      <c r="O31" s="13">
+        <v>0</v>
+      </c>
+      <c r="P31" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q31" s="13">
+        <v>0</v>
+      </c>
+      <c r="R31" s="13">
+        <v>0</v>
+      </c>
+      <c r="S31" s="13">
+        <v>0</v>
+      </c>
+      <c r="T31" s="13">
+        <v>0</v>
+      </c>
+      <c r="U31" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A32" t="s">
+        <v>87</v>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="F32" s="15">
+        <v>2700</v>
+      </c>
+      <c r="G32" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="H32" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="J32">
+        <v>5</v>
+      </c>
+      <c r="K32" s="14">
+        <v>0</v>
+      </c>
+      <c r="L32" s="13">
+        <v>0</v>
+      </c>
+      <c r="M32" s="13">
+        <v>0</v>
+      </c>
+      <c r="N32" s="13">
+        <v>0</v>
+      </c>
+      <c r="O32" s="13">
+        <v>0</v>
+      </c>
+      <c r="P32" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q32" s="13">
+        <v>0</v>
+      </c>
+      <c r="R32" s="13">
+        <v>0</v>
+      </c>
+      <c r="S32" s="13">
+        <v>0</v>
+      </c>
+      <c r="T32" s="13">
+        <v>0</v>
+      </c>
+      <c r="U32" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A33" t="s">
+        <v>88</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="F33" s="15">
+        <v>400</v>
+      </c>
+      <c r="G33" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="H33" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="J33">
+        <v>2</v>
+      </c>
+      <c r="K33" s="14">
+        <v>0</v>
+      </c>
+      <c r="L33" s="13">
+        <v>0</v>
+      </c>
+      <c r="M33" s="13">
+        <v>0</v>
+      </c>
+      <c r="N33" s="13">
+        <v>0</v>
+      </c>
+      <c r="O33" s="13">
+        <v>0</v>
+      </c>
+      <c r="P33" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q33" s="13">
+        <v>0</v>
+      </c>
+      <c r="R33" s="13">
+        <v>0</v>
+      </c>
+      <c r="S33" s="13">
+        <v>0</v>
+      </c>
+      <c r="T33" s="13">
+        <v>0</v>
+      </c>
+      <c r="U33" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A34" t="s">
+        <v>89</v>
+      </c>
+      <c r="B34" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="F34" s="15">
+        <v>1400</v>
+      </c>
+      <c r="G34" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="H34" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="J34">
+        <v>4</v>
+      </c>
+      <c r="K34" s="14">
+        <v>0</v>
+      </c>
+      <c r="L34" s="13">
+        <v>0</v>
+      </c>
+      <c r="M34" s="13">
+        <v>0</v>
+      </c>
+      <c r="N34" s="13">
+        <v>0</v>
+      </c>
+      <c r="O34" s="13">
+        <v>0</v>
+      </c>
+      <c r="P34" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q34" s="13">
+        <v>0</v>
+      </c>
+      <c r="R34" s="13">
+        <v>0</v>
+      </c>
+      <c r="S34" s="13">
+        <v>0</v>
+      </c>
+      <c r="T34" s="13">
+        <v>0</v>
+      </c>
+      <c r="U34" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A35" t="s">
+        <v>90</v>
+      </c>
+      <c r="B35" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="F35" s="15">
+        <v>25000</v>
+      </c>
+      <c r="G35" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="H35" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="J35">
+        <v>7</v>
+      </c>
+      <c r="K35" s="14">
+        <v>0</v>
+      </c>
+      <c r="L35" s="13">
+        <v>0</v>
+      </c>
+      <c r="M35" s="13">
+        <v>0</v>
+      </c>
+      <c r="N35" s="13">
+        <v>0</v>
+      </c>
+      <c r="O35" s="13">
+        <v>0</v>
+      </c>
+      <c r="P35" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q35" s="13">
+        <v>0</v>
+      </c>
+      <c r="R35" s="13">
+        <v>0</v>
+      </c>
+      <c r="S35" s="13">
+        <v>0</v>
+      </c>
+      <c r="T35" s="13">
+        <v>0</v>
+      </c>
+      <c r="U35" s="13">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -1834,7 +3373,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1846,7 +3385,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>